<commit_message>
Various updates made by 10/21
</commit_message>
<xml_diff>
--- a/samples/sample_consumption.xlsx
+++ b/samples/sample_consumption.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Month</t>
   </si>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -70,6 +70,11 @@
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -98,6 +103,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -314,6 +322,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="4.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
@@ -323,6 +334,9 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
@@ -332,7 +346,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="3">
-        <v>1481.0</v>
+        <v>1490.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>130.23</v>
       </c>
     </row>
     <row r="3">
@@ -343,7 +360,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="3">
-        <v>1317.0</v>
+        <v>1236.55</v>
+      </c>
+      <c r="D3" s="4">
+        <v>101.34</v>
       </c>
     </row>
     <row r="4">
@@ -356,6 +376,9 @@
       <c r="C4" s="3">
         <v>1664.0</v>
       </c>
+      <c r="D4" s="4">
+        <v>145.6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3">
@@ -367,6 +390,9 @@
       <c r="C5" s="3">
         <v>2294.0</v>
       </c>
+      <c r="D5" s="4">
+        <v>199.29</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3">
@@ -378,6 +404,9 @@
       <c r="C6" s="3">
         <v>1938.0</v>
       </c>
+      <c r="D6" s="4">
+        <v>178.62</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3">
@@ -389,6 +418,9 @@
       <c r="C7" s="3">
         <v>1829.0</v>
       </c>
+      <c r="D7" s="4">
+        <v>169.69</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
@@ -400,6 +432,9 @@
       <c r="C8" s="3">
         <v>3212.0</v>
       </c>
+      <c r="D8" s="4">
+        <v>220.41</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3">
@@ -411,6 +446,9 @@
       <c r="C9" s="3">
         <v>2641.0</v>
       </c>
+      <c r="D9" s="4">
+        <v>178.37</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3">
@@ -422,6 +460,9 @@
       <c r="C10" s="3">
         <v>2194.0</v>
       </c>
+      <c r="D10" s="4">
+        <v>130.65</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3">
@@ -433,6 +474,9 @@
       <c r="C11" s="3">
         <v>1771.0</v>
       </c>
+      <c r="D11" s="4">
+        <v>125.62</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3">
@@ -444,6 +488,9 @@
       <c r="C12" s="3">
         <v>1678.0</v>
       </c>
+      <c r="D12" s="4">
+        <v>120.54</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3">
@@ -453,10 +500,19 @@
         <v>13</v>
       </c>
       <c r="C13" s="3">
-        <v>1713.0</v>
+        <v>1713.23</v>
+      </c>
+      <c r="D13" s="4">
+        <v>135.34</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between .1 and 10000" sqref="C2:C13">
+      <formula1>0.1</formula1>
+      <formula2>10000.0</formula2>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>